<commit_message>
Rename script-48, as its just a demo recording, not then tape player
</commit_message>
<xml_diff>
--- a/Demo/ManiacMansion-Demo.xlsx
+++ b/Demo/ManiacMansion-Demo.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.200\home\Archive\Robs Projects\Maniac.Mansion.Disassembly\Demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.200\home\Projects\Maniac.Mansion.Disassembly\Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="0" windowWidth="3660" windowHeight="1965" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="22320" windowHeight="9468" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="3" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Handle Doorbell</t>
   </si>
   <si>
-    <t>Tape Player: Play Tape</t>
-  </si>
-  <si>
     <t>Door: Close</t>
   </si>
   <si>
@@ -505,12 +502,15 @@
   </si>
   <si>
     <t>Phone: LucasFilm Line</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Demo: Advertisement Recording</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -848,217 +848,217 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="5.88671875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>0</v>
       </c>
       <c r="B2" s="5"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>13</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1074,236 +1074,236 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>3</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>6</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>7</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>8</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>10</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>31</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>33</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>36</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>37</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>43</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>45</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>49</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -1322,14 +1322,14 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1345,22 +1345,22 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1138</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1373,354 +1373,354 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>39</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>40</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>41</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>44</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>45</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>46</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>48</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>49</v>
       </c>
@@ -1744,215 +1744,215 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="4"/>
-    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="4"/>
+    <col min="3" max="3" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="F1" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>48</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>76</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>91</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>92</v>
       </c>
       <c r="C6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" t="s">
         <v>151</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>152</v>
       </c>
-      <c r="F6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>97</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>99</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>136</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>78</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>96</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>68</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>29</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>148</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>149</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1971,211 +1971,211 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>112</v>
-      </c>
-      <c r="C1" s="9"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>113</v>
       </c>
       <c r="B2" s="11">
         <v>4</v>
       </c>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="11">
         <v>5</v>
       </c>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4" s="11">
         <v>6</v>
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" s="11">
         <v>7</v>
       </c>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
       <c r="B6" s="11"/>
       <c r="C6" s="9"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>117</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C8" s="9"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>118</v>
       </c>
       <c r="B9" s="11">
         <v>0</v>
       </c>
       <c r="C9" s="11"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B10" s="11">
         <v>1</v>
       </c>
       <c r="C10" s="11"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B11" s="11">
         <v>2</v>
       </c>
       <c r="C11" s="11"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B12" s="11">
         <v>3</v>
       </c>
       <c r="C12" s="11"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B13" s="11">
         <v>4</v>
       </c>
       <c r="C13" s="11"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B14" s="11">
         <v>5</v>
       </c>
       <c r="C14" s="11"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B15" s="11">
         <v>6</v>
       </c>
       <c r="C15" s="11"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B16" s="11">
         <v>7</v>
       </c>
       <c r="C16" s="11"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B17" s="11">
         <v>8</v>
       </c>
       <c r="C17" s="11"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B18" s="11">
         <v>9</v>
       </c>
       <c r="C18" s="11"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="C19" s="11"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C19" s="11"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="B20" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="C20" s="11"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C20" s="11"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="B21" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="C21" s="11"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C21" s="11"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="B22" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="C22" s="11"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="C22" s="11"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="B23" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="C23" s="11"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C23" s="11"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="B24" s="11" t="s">
         <v>138</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>139</v>
       </c>
       <c r="C24" s="11"/>
     </row>
@@ -2192,50 +2192,50 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="9"/>
-    <col min="3" max="3" width="13.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="2" width="9.109375" style="9"/>
+    <col min="3" max="3" width="13.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>4</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add comments to glass jar script, Add variable to spreadsheet, fix script page for demo
</commit_message>
<xml_diff>
--- a/Demo/ManiacMansion-Demo.xlsx
+++ b/Demo/ManiacMansion-Demo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="22320" windowHeight="9468" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="22320" windowHeight="9468" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="3" r:id="rId1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="158">
-  <si>
-    <t>Script Number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="161">
   <si>
     <t>Handle Doorbell</t>
   </si>
@@ -330,9 +327,6 @@
     <t>Library</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>Pool Area</t>
   </si>
   <si>
@@ -504,7 +498,22 @@
     <t>Phone: LucasFilm Line</t>
   </si>
   <si>
-    <t xml:space="preserve"> Demo: Advertisement Recording</t>
+    <t>Cutscene</t>
+  </si>
+  <si>
+    <t>Started By</t>
+  </si>
+  <si>
+    <t>Input Variable</t>
+  </si>
+  <si>
+    <t>Demo: Advertisement Recording</t>
+  </si>
+  <si>
+    <t>Var[76] Death Method</t>
+  </si>
+  <si>
+    <t>Var[77] Actor</t>
   </si>
 </sst>
 </file>
@@ -548,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -562,6 +571,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -857,10 +868,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -874,7 +885,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -882,7 +893,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -890,7 +901,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -898,7 +909,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -906,7 +917,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -914,7 +925,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -922,7 +933,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -930,7 +941,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -938,7 +949,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -946,7 +957,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -954,7 +965,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -962,7 +973,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -970,7 +981,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -978,7 +989,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -986,7 +997,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -994,7 +1005,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -1002,7 +1013,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -1010,7 +1021,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -1018,7 +1029,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -1026,7 +1037,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -1034,7 +1045,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -1042,7 +1053,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -1050,7 +1061,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -1058,7 +1069,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1071,7 +1082,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1083,16 +1094,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1100,13 +1111,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1114,13 +1125,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1128,13 +1139,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>99</v>
+        <v>12</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1142,13 +1153,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1156,13 +1167,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1170,13 +1181,13 @@
         <v>8</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1184,13 +1195,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1198,13 +1209,13 @@
         <v>31</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1212,13 +1223,13 @@
         <v>33</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1226,13 +1237,13 @@
         <v>36</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1240,13 +1251,13 @@
         <v>37</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1254,13 +1265,13 @@
         <v>43</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1268,13 +1279,13 @@
         <v>45</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1282,13 +1293,13 @@
         <v>49</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1329,7 +1340,7 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1352,7 +1363,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1360,7 +1371,7 @@
         <v>1138</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1371,307 +1382,406 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
+      <c r="B4" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C4" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
+      <c r="B5" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
+      <c r="B10" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
+      <c r="B11" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>12</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>13</v>
       </c>
+      <c r="B13" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>14</v>
       </c>
+      <c r="B14" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>15</v>
       </c>
+      <c r="B15" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>16</v>
       </c>
+      <c r="B16" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>17</v>
       </c>
+      <c r="B17" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>18</v>
       </c>
+      <c r="B18" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>19</v>
       </c>
+      <c r="B19" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>20</v>
       </c>
+      <c r="B20" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>21</v>
       </c>
+      <c r="B21" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>22</v>
       </c>
+      <c r="B22" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>23</v>
       </c>
+      <c r="B23" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="E24" t="s">
+        <v>159</v>
+      </c>
+      <c r="F24" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>30</v>
       </c>
+      <c r="B26" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>31</v>
       </c>
+      <c r="B27" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C27" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>32</v>
       </c>
+      <c r="B28" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>33</v>
       </c>
+      <c r="B29" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>33</v>
       </c>
+      <c r="B30" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C30" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>36</v>
       </c>
+      <c r="B31" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>37</v>
       </c>
+      <c r="B32" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>38</v>
       </c>
+      <c r="B33" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>39</v>
       </c>
+      <c r="B34" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C34" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>40</v>
       </c>
+      <c r="B35" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C35" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1679,10 +1789,10 @@
         <v>41</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1690,42 +1800,54 @@
         <v>44</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>45</v>
       </c>
+      <c r="B38" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="C38" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>46</v>
       </c>
+      <c r="B39" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="C39" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>48</v>
       </c>
+      <c r="B40" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C40" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>49</v>
       </c>
+      <c r="B41" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1741,7 +1863,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1758,22 +1880,22 @@
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="F1" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1781,19 +1903,19 @@
         <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1801,7 +1923,7 @@
         <v>48</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1809,22 +1931,22 @@
         <v>76</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1832,16 +1954,16 @@
         <v>91</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1849,13 +1971,13 @@
         <v>92</v>
       </c>
       <c r="C6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F6" t="s">
         <v>150</v>
-      </c>
-      <c r="E6" t="s">
-        <v>151</v>
-      </c>
-      <c r="F6" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1863,7 +1985,7 @@
         <v>97</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1871,7 +1993,7 @@
         <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1879,7 +2001,7 @@
         <v>99</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1887,7 +2009,7 @@
         <v>136</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1895,13 +2017,13 @@
         <v>78</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1909,13 +2031,13 @@
         <v>96</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1923,7 +2045,7 @@
         <v>68</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1932,14 +2054,14 @@
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
@@ -1949,10 +2071,10 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1978,16 +2100,16 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B2" s="11">
         <v>4</v>
@@ -1996,7 +2118,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B3" s="11">
         <v>5</v>
@@ -2005,7 +2127,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B4" s="11">
         <v>6</v>
@@ -2014,7 +2136,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B5" s="11">
         <v>7</v>
@@ -2028,16 +2150,16 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B9" s="11">
         <v>0</v>
@@ -2046,7 +2168,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B10" s="11">
         <v>1</v>
@@ -2055,7 +2177,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B11" s="11">
         <v>2</v>
@@ -2064,7 +2186,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B12" s="11">
         <v>3</v>
@@ -2073,7 +2195,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B13" s="11">
         <v>4</v>
@@ -2082,7 +2204,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B14" s="11">
         <v>5</v>
@@ -2091,7 +2213,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B15" s="11">
         <v>6</v>
@@ -2100,7 +2222,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B16" s="11">
         <v>7</v>
@@ -2109,7 +2231,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B17" s="11">
         <v>8</v>
@@ -2118,7 +2240,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B18" s="11">
         <v>9</v>
@@ -2127,55 +2249,55 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C19" s="11"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C20" s="11"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C21" s="11"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C22" s="11"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C23" s="11"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C24" s="11"/>
     </row>
@@ -2189,7 +2311,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2201,16 +2323,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2218,13 +2340,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>141</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2232,10 +2354,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retail & Demo comment improvements
</commit_message>
<xml_diff>
--- a/Demo/ManiacMansion-Demo.xlsx
+++ b/Demo/ManiacMansion-Demo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="22320" windowHeight="9468" activeTab="4"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="20340" windowHeight="12960"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="3" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Variables" sheetId="2" r:id="rId6"/>
     <sheet name="Values" sheetId="6" r:id="rId7"/>
     <sheet name="BitVars" sheetId="7" r:id="rId8"/>
+    <sheet name="Actor BitVars" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="184">
   <si>
     <t>Handle Doorbell</t>
   </si>
@@ -514,6 +515,75 @@
   </si>
   <si>
     <t>Var[77] Actor</t>
+  </si>
+  <si>
+    <t>Var</t>
+  </si>
+  <si>
+    <t>0x01</t>
+  </si>
+  <si>
+    <t>Kid is strong (Hunk-O-Matic used)</t>
+  </si>
+  <si>
+    <t>kActorMiscFlagStrong</t>
+  </si>
+  <si>
+    <t>0x02</t>
+  </si>
+  <si>
+    <t>Kid is green tentacle's friend (recording contract)</t>
+  </si>
+  <si>
+    <t>kActorMiscFlagGTFriend</t>
+  </si>
+  <si>
+    <t>0x04</t>
+  </si>
+  <si>
+    <t>Kid knows publisher's address (watched TV)</t>
+  </si>
+  <si>
+    <t>kActorMiscFlagWatchedTV</t>
+  </si>
+  <si>
+    <t>0x08</t>
+  </si>
+  <si>
+    <t>Kid is not Weird Ed's friend</t>
+  </si>
+  <si>
+    <t>kActorMiscFlagEdsEnemy</t>
+  </si>
+  <si>
+    <t>0x10</t>
+  </si>
+  <si>
+    <t>kActorMiscFlag_10</t>
+  </si>
+  <si>
+    <t>0x20</t>
+  </si>
+  <si>
+    <t>kActorMiscFlag_20</t>
+  </si>
+  <si>
+    <t>0x40</t>
+  </si>
+  <si>
+    <t>Kid stops moving</t>
+  </si>
+  <si>
+    <t>kActorMiscFlagFreeze</t>
+  </si>
+  <si>
+    <t>0x80</t>
+  </si>
+  <si>
+    <t>Kid is invisible (dead or in radiation suit)</t>
+  </si>
+  <si>
+    <t>kActorMiscFlagHide</t>
   </si>
 </sst>
 </file>
@@ -855,7 +925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -1384,7 +1454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -2363,4 +2433,120 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="13"/>
+    <col min="2" max="2" width="45.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add more variables, improve comments
</commit_message>
<xml_diff>
--- a/Demo/ManiacMansion-Demo.xlsx
+++ b/Demo/ManiacMansion-Demo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="5652" windowHeight="888" activeTab="5"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="14172" windowHeight="10860" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="317">
   <si>
     <t>Handle Doorbell</t>
   </si>
@@ -972,6 +972,18 @@
   </si>
   <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>Stamps Taken</t>
+  </si>
+  <si>
+    <t>1 = Stamps Taken</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1027,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1031,6 +1043,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1656,7 +1669,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1901,10 +1914,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1935,6 +1948,14 @@
       </c>
       <c r="B3" t="s">
         <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -3657,7 +3678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -4133,10 +4154,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4362,90 +4383,108 @@
       </c>
     </row>
     <row r="22" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13">
+      <c r="A22" s="15">
+        <v>81</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="13">
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24">
         <v>91</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>5</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>151</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F24" t="s">
         <v>152</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G24" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
-        <v>92</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>88</v>
+        <v>148</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>90</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
+        <v>96</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
         <v>97</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="4" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
+    <row r="28" spans="1:9" s="4" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
         <v>98</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="12">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="12">
         <v>99</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12" t="s">
+      <c r="B29" s="12"/>
+      <c r="C29" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30">
         <v>136</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add C64 disk layout Add V0 Demo Room Map Add more sounds/vars to spreadsheet
</commit_message>
<xml_diff>
--- a/Demo/ManiacMansion-Demo.xlsx
+++ b/Demo/ManiacMansion-Demo.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.200\home\Projects\Maniac.Mansion.Disassembly\Demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Desktop\Maniac.Mansion.Disassembly\Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="14172" windowHeight="10860" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="1932" yWindow="0" windowWidth="14172" windowHeight="10860" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="325">
   <si>
     <t>Handle Doorbell</t>
   </si>
@@ -984,6 +984,30 @@
   </si>
   <si>
     <t>1 = Stamps Taken</t>
+  </si>
+  <si>
+    <t>Var[92]</t>
+  </si>
+  <si>
+    <t>Outputs</t>
+  </si>
+  <si>
+    <t>1 = Flashlight</t>
+  </si>
+  <si>
+    <t>2 = Light on</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Var[48]</t>
+  </si>
+  <si>
+    <t>0 = Pin Correct</t>
+  </si>
+  <si>
+    <t>1 = Pin Wrong</t>
   </si>
 </sst>
 </file>
@@ -3676,10 +3700,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3690,9 +3714,12 @@
     <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>80</v>
       </c>
@@ -3708,8 +3735,14 @@
       <c r="E1" s="14" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H1" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3720,7 +3753,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -3731,7 +3764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -3742,7 +3775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -3753,7 +3786,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -3764,7 +3797,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -3775,7 +3808,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -3786,7 +3819,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -3797,7 +3830,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
@@ -3808,7 +3841,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12</v>
       </c>
@@ -3819,7 +3852,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>13</v>
       </c>
@@ -3830,7 +3863,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>14</v>
       </c>
@@ -3841,7 +3874,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>15</v>
       </c>
@@ -3852,7 +3885,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>16</v>
       </c>
@@ -3863,7 +3896,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>17</v>
       </c>
@@ -3874,7 +3907,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>18</v>
       </c>
@@ -3884,8 +3917,17 @@
       <c r="C18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>322</v>
+      </c>
+      <c r="J18" t="s">
+        <v>323</v>
+      </c>
+      <c r="K18" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>19</v>
       </c>
@@ -3895,8 +3937,20 @@
       <c r="C19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>317</v>
+      </c>
+      <c r="J19" t="s">
+        <v>145</v>
+      </c>
+      <c r="K19" t="s">
+        <v>319</v>
+      </c>
+      <c r="L19" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>20</v>
       </c>
@@ -3907,7 +3961,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>21</v>
       </c>
@@ -3918,7 +3972,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>22</v>
       </c>
@@ -3929,7 +3983,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>23</v>
       </c>
@@ -3940,7 +3994,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>24</v>
       </c>
@@ -3957,7 +4011,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>25</v>
       </c>
@@ -3968,7 +4022,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>30</v>
       </c>
@@ -3979,7 +4033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>31</v>
       </c>
@@ -3990,7 +4044,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>32</v>
       </c>
@@ -4001,7 +4055,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>33</v>
       </c>
@@ -4012,7 +4066,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>33</v>
       </c>
@@ -4023,7 +4077,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>36</v>
       </c>
@@ -4034,7 +4088,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>37</v>
       </c>
@@ -4149,6 +4203,7 @@
     <sortCondition ref="A3:A38"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4156,8 +4211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:I22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>